<commit_message>
Fixed accounting error in the summary file.
</commit_message>
<xml_diff>
--- a/Device Interaction/Automation/Summary Statistics - Device - Automation.xlsx
+++ b/Device Interaction/Automation/Summary Statistics - Device - Automation.xlsx
@@ -371,7 +371,7 @@
       </c>
       <c r="D4" s="9">
         <f>F29+G29</f>
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="1"/>
@@ -449,6 +449,10 @@
     <row r="8">
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
+      <c r="D8">
+        <f>sum(D4:E6)</f>
+        <v>1263</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -722,7 +726,7 @@
         <v>28</v>
       </c>
       <c r="F27" s="15">
-        <v>157.0</v>
+        <v>152.0</v>
       </c>
       <c r="G27" s="15">
         <v>5.0</v>
@@ -768,7 +772,7 @@
       <c r="D29" s="1"/>
       <c r="F29" s="21">
         <f t="shared" ref="F29:K29" si="3">sum(F15:F28)</f>
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="G29" s="21">
         <f t="shared" si="3"/>
@@ -831,7 +835,7 @@
       </c>
       <c r="C33" s="23">
         <f>D4/(D4+G6+H6)</f>
-        <v>0.9738292011</v>
+        <v>0.9736477115</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>

</xml_diff>

<commit_message>
Fixed more accounting errors.
</commit_message>
<xml_diff>
--- a/Device Interaction/Automation/Summary Statistics - Device - Automation.xlsx
+++ b/Device Interaction/Automation/Summary Statistics - Device - Automation.xlsx
@@ -9,6 +9,28 @@
   <definedNames/>
   <calcPr/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="G6">
+      <text>
+        <t xml:space="preserve">12 out of 16 are actual conflicts
+4 are found as non conflicts</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="H6">
+      <text>
+        <t xml:space="preserve">25 out of 33 are actual conflicts
+8 are found as non conflicts</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -130,6 +152,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10.0"/>
@@ -278,7 +303,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="46" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
@@ -371,7 +396,7 @@
       </c>
       <c r="D4" s="9">
         <f>F29+G29</f>
-        <v>702</v>
+        <v>717</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="1"/>
@@ -388,11 +413,11 @@
       </c>
       <c r="D5" s="13">
         <f t="shared" ref="D5:E5" si="1">H29</f>
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E5" s="14">
         <f t="shared" si="1"/>
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="15" t="s">
@@ -412,7 +437,7 @@
       </c>
       <c r="D6" s="13">
         <f t="shared" ref="D6:E6" si="2">J29</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="14">
         <f t="shared" si="2"/>
@@ -420,13 +445,13 @@
       </c>
       <c r="F6" s="1">
         <f>E5+E6</f>
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="G6" s="15">
-        <v>9.0</v>
+        <v>12.0</v>
       </c>
       <c r="H6" s="15">
-        <v>10.0</v>
+        <v>25.0</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -726,20 +751,18 @@
         <v>28</v>
       </c>
       <c r="F27" s="15">
-        <v>152.0</v>
+        <v>164.0</v>
       </c>
       <c r="G27" s="15">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="H27" s="15">
-        <v>19.0</v>
+        <v>8.0</v>
       </c>
       <c r="I27" s="15">
-        <v>32.0</v>
-      </c>
-      <c r="J27" s="15">
-        <v>1.0</v>
-      </c>
+        <v>29.0</v>
+      </c>
+      <c r="J27" s="15"/>
       <c r="K27" s="15">
         <v>1.0</v>
       </c>
@@ -772,23 +795,23 @@
       <c r="D29" s="1"/>
       <c r="F29" s="21">
         <f t="shared" ref="F29:K29" si="3">sum(F15:F28)</f>
-        <v>667</v>
+        <v>679</v>
       </c>
       <c r="G29" s="21">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H29" s="21">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="I29" s="21">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J29" s="21">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K29" s="21">
         <f t="shared" si="3"/>
@@ -835,7 +858,7 @@
       </c>
       <c r="C33" s="23">
         <f>D4/(D4+G6+H6)</f>
-        <v>0.9736477115</v>
+        <v>0.950928382</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -8592,9 +8615,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B31"/>
+    <hyperlink r:id="rId2" ref="B31"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -8709,7 +8733,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="24">
-        <v>8.101851851851852E-5</v>
+        <v>9.259259259259259E-5</v>
       </c>
     </row>
     <row r="15">
@@ -8726,7 +8750,7 @@
       </c>
       <c r="C17" s="27">
         <f>average(C2:C15)</f>
-        <v>0.000306712963</v>
+        <v>0.0003078703704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified results after re-running executions due to serialization ID assignment bug fix.
</commit_message>
<xml_diff>
--- a/Device Interaction/Automation/Summary Statistics - Device - Automation.xlsx
+++ b/Device Interaction/Automation/Summary Statistics - Device - Automation.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Interaction</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Excluded</t>
+  </si>
+  <si>
+    <t>False Positives</t>
   </si>
   <si>
     <t>Conflict - Conflict</t>
@@ -395,10 +398,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="9">
-        <f>F29+G29</f>
-        <v>717</v>
-      </c>
-      <c r="E4" s="10"/>
+        <f t="shared" ref="D4:E4" si="1">F29</f>
+        <v>679</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -412,11 +418,11 @@
         <v>4</v>
       </c>
       <c r="D5" s="13">
-        <f t="shared" ref="D5:E5" si="1">H29</f>
+        <f t="shared" ref="D5:E5" si="2">H29</f>
         <v>33</v>
       </c>
       <c r="E5" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>101</v>
       </c>
       <c r="F5" s="1"/>
@@ -436,11 +442,11 @@
         <v>8</v>
       </c>
       <c r="D6" s="13">
-        <f t="shared" ref="D6:E6" si="2">J29</f>
+        <f t="shared" ref="D6:E6" si="3">J29</f>
         <v>16</v>
       </c>
       <c r="E6" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>396</v>
       </c>
       <c r="F6" s="1">
@@ -496,6 +502,12 @@
     </row>
     <row r="10">
       <c r="C10" s="12"/>
+      <c r="D10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.0</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -535,27 +547,27 @@
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="F14" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F15" s="15">
         <v>8.0</v>
@@ -574,7 +586,7 @@
     </row>
     <row r="16">
       <c r="B16" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -586,7 +598,7 @@
     </row>
     <row r="17">
       <c r="B17" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" s="15">
         <v>6.0</v>
@@ -601,7 +613,7 @@
     </row>
     <row r="18">
       <c r="B18" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F18" s="15">
         <v>7.0</v>
@@ -618,7 +630,7 @@
     </row>
     <row r="19">
       <c r="B19" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F19" s="15">
         <v>18.0</v>
@@ -639,7 +651,7 @@
     </row>
     <row r="20">
       <c r="B20" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F20" s="15">
         <v>72.0</v>
@@ -660,7 +672,7 @@
     </row>
     <row r="21">
       <c r="B21" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -673,7 +685,7 @@
     </row>
     <row r="22">
       <c r="B22" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -686,7 +698,7 @@
     </row>
     <row r="23">
       <c r="B23" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F23" s="15">
         <v>3.0</v>
@@ -699,7 +711,7 @@
     </row>
     <row r="24">
       <c r="B24" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -712,7 +724,7 @@
     </row>
     <row r="25">
       <c r="B25" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F25" s="15">
         <v>16.0</v>
@@ -733,7 +745,7 @@
     </row>
     <row r="26">
       <c r="B26" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F26" s="15">
         <v>6.0</v>
@@ -748,7 +760,7 @@
     </row>
     <row r="27">
       <c r="B27" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F27" s="15">
         <v>164.0</v>
@@ -769,7 +781,7 @@
     </row>
     <row r="28">
       <c r="B28" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -794,27 +806,27 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="F29" s="21">
-        <f t="shared" ref="F29:K29" si="3">sum(F15:F28)</f>
+        <f t="shared" ref="F29:K29" si="4">sum(F15:F28)</f>
         <v>679</v>
       </c>
       <c r="G29" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="H29" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="I29" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
       <c r="J29" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="K29" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>396</v>
       </c>
     </row>
@@ -828,7 +840,7 @@
     </row>
     <row r="31">
       <c r="B31" s="22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -839,10 +851,10 @@
     </row>
     <row r="32">
       <c r="B32" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" s="23">
-        <f>D4/(D4+E4)</f>
+        <f>(D4+E4)/(D4+E4+E10)</f>
         <v>1</v>
       </c>
       <c r="F32" s="1"/>
@@ -854,10 +866,10 @@
     </row>
     <row r="33">
       <c r="B33" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33" s="23">
-        <f>D4/(D4+G6+H6)</f>
+        <f>(D4+E4)/(D4+E4+G6+H6)</f>
         <v>0.950928382</v>
       </c>
       <c r="F33" s="1"/>
@@ -869,10 +881,10 @@
     </row>
     <row r="34">
       <c r="B34" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34" s="23">
-        <f>F6/(F6+E4)</f>
+        <f>F6/(F6+E10)</f>
         <v>1</v>
       </c>
       <c r="F34" s="1"/>
@@ -940,7 +952,7 @@
     </row>
     <row r="42">
       <c r="B42" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -8637,12 +8649,12 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="24">
         <v>4.7453703703703704E-4</v>
@@ -8650,13 +8662,13 @@
     </row>
     <row r="3">
       <c r="B3" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="25"/>
     </row>
     <row r="4">
       <c r="B4" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="24">
         <v>5.787037037037037E-4</v>
@@ -8664,7 +8676,7 @@
     </row>
     <row r="5">
       <c r="B5" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="24">
         <v>1.8518518518518518E-4</v>
@@ -8672,7 +8684,7 @@
     </row>
     <row r="6">
       <c r="B6" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="24">
         <v>1.273148148148148E-4</v>
@@ -8680,7 +8692,7 @@
     </row>
     <row r="7">
       <c r="B7" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="24">
         <v>1.7361111111111112E-4</v>
@@ -8688,19 +8700,19 @@
     </row>
     <row r="8">
       <c r="B8" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="25"/>
     </row>
     <row r="9">
       <c r="B9" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="25"/>
     </row>
     <row r="10">
       <c r="B10" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="24">
         <v>5.902777777777778E-4</v>
@@ -8708,13 +8720,13 @@
     </row>
     <row r="11">
       <c r="B11" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="25"/>
     </row>
     <row r="12">
       <c r="B12" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="24">
         <v>5.208333333333333E-4</v>
@@ -8722,7 +8734,7 @@
     </row>
     <row r="13">
       <c r="B13" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="26">
         <v>6.944444444444444E-5</v>
@@ -8730,7 +8742,7 @@
     </row>
     <row r="14">
       <c r="B14" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="24">
         <v>9.259259259259259E-5</v>
@@ -8738,7 +8750,7 @@
     </row>
     <row r="15">
       <c r="B15" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="24">
         <v>2.662037037037037E-4</v>
@@ -8746,7 +8758,7 @@
     </row>
     <row r="17">
       <c r="B17" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="27">
         <f>average(C2:C15)</f>

</xml_diff>